<commit_message>
mail sur les questions pour les designer
</commit_message>
<xml_diff>
--- a/90Outils/process front-controller.xlsx
+++ b/90Outils/process front-controller.xlsx
@@ -199,12 +199,27 @@
         </r>
       </text>
     </comment>
+    <comment ref="D115" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">remarque sur le controleur, role, elt en entrée, elts en sortie ….. :
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="62">
   <si>
     <t xml:space="preserve">ecran : </t>
   </si>
@@ -381,6 +396,42 @@
   </si>
   <si>
     <t xml:space="preserve">liste des question rattachées à ce QCM : </t>
+  </si>
+  <si>
+    <t>Description de la question, avec les réponses proposées</t>
+  </si>
+  <si>
+    <t>le nom du Designer si ce n'est pas l'utilisateur en cours</t>
+  </si>
+  <si>
+    <t>Fermer</t>
+  </si>
+  <si>
+    <t>Signaler ou envoyer un mail</t>
+  </si>
+  <si>
+    <t>detail de la question, fenetre interne de type "FanzyBox"</t>
+  </si>
+  <si>
+    <t>fenetre appelante</t>
+  </si>
+  <si>
+    <t>"/MailEngine"</t>
+  </si>
+  <si>
+    <t>MailEngineController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uniquement visible pour </t>
+  </si>
+  <si>
+    <t>questions dont pas designer</t>
+  </si>
+  <si>
+    <t>génération du mail dans une fenetre externe</t>
+  </si>
+  <si>
+    <t>en revanche, cette derniere ne se ferme pas en auto :-(</t>
   </si>
 </sst>
 </file>
@@ -760,7 +811,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -774,20 +825,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -797,6 +836,73 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -834,18 +940,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -854,32 +955,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -896,36 +976,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2559,6 +2617,464 @@
           <a:solidFill>
             <a:srgbClr val="FF0000"/>
           </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>504266</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>537882</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Connecteur droit avec flèche 34"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="12606619" y="20842941"/>
+          <a:ext cx="33616" cy="2196353"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>78441</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>638738</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Connecteur droit avec flèche 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5031441" y="22277294"/>
+          <a:ext cx="4403915" cy="437030"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>661147</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>163608</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Connecteur droit avec flèche 38"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2554941" y="20898971"/>
+          <a:ext cx="952500" cy="914402"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>459441</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>67237</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Connecteur droit avec flèche 42"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12942794" y="18859500"/>
+          <a:ext cx="1299882" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>73959</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>107579</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>459441</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="Connecteur droit avec flèche 46"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12837459" y="12557314"/>
+          <a:ext cx="1405217" cy="4480"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>582706</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>459441</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Connecteur droit avec flèche 48"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11362765" y="16259735"/>
+          <a:ext cx="2879911" cy="22412"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>560294</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>560296</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Connecteur droit avec flèche 50"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11340353" y="16013206"/>
+          <a:ext cx="2" cy="280146"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>448236</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>156883</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>459441</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="65" name="Connecteur droit avec flèche 64"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14231471" y="12606618"/>
+          <a:ext cx="11205" cy="9659470"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>40343</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>454960</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Connecteur droit avec flèche 68"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13435853" y="22272814"/>
+          <a:ext cx="802342" cy="15686"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
           <a:tailEnd type="arrow"/>
         </a:ln>
       </xdr:spPr>
@@ -2869,10 +3385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AA107"/>
+  <dimension ref="B1:AA122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.85546875" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -2889,61 +3405,61 @@
       </c>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
     </row>
     <row r="9" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="45"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="58"/>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="60"/>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="AA13" t="s">
@@ -2959,107 +3475,107 @@
       <c r="J15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K15" s="48" t="s">
+      <c r="K15" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="16"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="12"/>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="J16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="16"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="12"/>
     </row>
     <row r="17" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="44"/>
-      <c r="F17" s="45"/>
-      <c r="J17" s="26" t="s">
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
+      <c r="J17" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="17" t="s">
+      <c r="K17" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="19"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="46"/>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="10"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="22"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="60"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="48"/>
+      <c r="S18" s="49"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="25"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="70"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="52"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
       <c r="J20" s="1"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -3073,20 +3589,20 @@
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="J21" s="1"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="31"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="15"/>
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="E22" s="43"/>
+      <c r="E22" s="27"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="32"/>
+      <c r="K22" s="16"/>
       <c r="L22" s="2" t="s">
         <v>13</v>
       </c>
@@ -3095,72 +3611,72 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
-      <c r="R22" s="33"/>
+      <c r="R22" s="17"/>
       <c r="S22" s="3"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="J23" s="1"/>
-      <c r="K23" s="32"/>
+      <c r="K23" s="16"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
-      <c r="R23" s="33"/>
+      <c r="R23" s="17"/>
       <c r="S23" s="3"/>
     </row>
     <row r="24" spans="3:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="44"/>
-      <c r="F24" s="45"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="58"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="41" t="s">
+      <c r="K24" s="16"/>
+      <c r="L24" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="M24" s="42"/>
+      <c r="M24" s="26"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
-      <c r="R24" s="33"/>
+      <c r="R24" s="17"/>
       <c r="S24" s="3"/>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C25" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D25" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="35"/>
-      <c r="R25" s="36"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="20"/>
       <c r="S25" s="3"/>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C26" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="38"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
       <c r="J26" s="1"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -3176,17 +3692,17 @@
       <c r="C27" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
       <c r="J27" s="1"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="41" t="s">
+      <c r="L27" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="42"/>
+      <c r="M27" s="26"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -3220,27 +3736,27 @@
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.25">
       <c r="J30" s="1"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="30"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="31"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="15"/>
       <c r="S30" s="3"/>
     </row>
     <row r="31" spans="3:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="44" t="s">
+      <c r="D31" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="44"/>
-      <c r="F31" s="45"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="58"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="32"/>
+      <c r="K31" s="16"/>
       <c r="L31" s="2" t="s">
         <v>16</v>
       </c>
@@ -3249,200 +3765,200 @@
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
-      <c r="R31" s="33"/>
+      <c r="R31" s="17"/>
       <c r="S31" s="3"/>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C32" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="39" t="s">
+      <c r="D32" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="40"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="24"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="32"/>
+      <c r="K32" s="16"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
-      <c r="R32" s="33"/>
+      <c r="R32" s="17"/>
       <c r="S32" s="3"/>
     </row>
     <row r="33" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C33" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="37" t="s">
+      <c r="D33" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="37"/>
-      <c r="F33" s="38"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="22"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="32"/>
-      <c r="M33" s="42"/>
+      <c r="K33" s="16"/>
+      <c r="M33" s="26"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
-      <c r="R33" s="33"/>
+      <c r="R33" s="17"/>
       <c r="S33" s="3"/>
     </row>
     <row r="34" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C34" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="46" t="s">
+      <c r="D34" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
       <c r="J34" s="1"/>
-      <c r="K34" s="32"/>
+      <c r="K34" s="16"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="O34" s="41" t="s">
+      <c r="O34" s="25" t="s">
         <v>17</v>
       </c>
       <c r="P34" s="2"/>
-      <c r="Q34" s="41" t="s">
+      <c r="Q34" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="R34" s="33"/>
+      <c r="R34" s="17"/>
       <c r="S34" s="3"/>
     </row>
     <row r="35" spans="3:19" x14ac:dyDescent="0.25">
       <c r="J35" s="1"/>
-      <c r="K35" s="32"/>
+      <c r="K35" s="16"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
-      <c r="R35" s="33"/>
+      <c r="R35" s="17"/>
       <c r="S35" s="3"/>
     </row>
     <row r="36" spans="3:19" x14ac:dyDescent="0.25">
       <c r="J36" s="1"/>
-      <c r="K36" s="32"/>
+      <c r="K36" s="16"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
-      <c r="R36" s="33"/>
+      <c r="R36" s="17"/>
       <c r="S36" s="3"/>
     </row>
     <row r="37" spans="3:19" x14ac:dyDescent="0.25">
       <c r="J37" s="1"/>
-      <c r="K37" s="32"/>
+      <c r="K37" s="16"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
-      <c r="R37" s="33"/>
+      <c r="R37" s="17"/>
       <c r="S37" s="3"/>
     </row>
     <row r="38" spans="3:19" x14ac:dyDescent="0.25">
       <c r="J38" s="1"/>
-      <c r="K38" s="32"/>
+      <c r="K38" s="16"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
-      <c r="R38" s="33"/>
+      <c r="R38" s="17"/>
       <c r="S38" s="3"/>
     </row>
     <row r="39" spans="3:19" x14ac:dyDescent="0.25">
       <c r="J39" s="1"/>
-      <c r="K39" s="32"/>
+      <c r="K39" s="16"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
-      <c r="R39" s="33"/>
+      <c r="R39" s="17"/>
       <c r="S39" s="3"/>
     </row>
     <row r="40" spans="3:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C40" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D40" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="E40" s="44"/>
-      <c r="F40" s="45"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="58"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="32"/>
+      <c r="K40" s="16"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
-      <c r="R40" s="33"/>
+      <c r="R40" s="17"/>
       <c r="S40" s="3"/>
     </row>
     <row r="41" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C41" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="39" t="s">
+      <c r="D41" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="39"/>
-      <c r="F41" s="40"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="24"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="32"/>
+      <c r="K41" s="16"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
-      <c r="R41" s="33"/>
+      <c r="R41" s="17"/>
       <c r="S41" s="3"/>
     </row>
     <row r="42" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C42" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="37" t="s">
+      <c r="D42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="37"/>
-      <c r="F42" s="38"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="22"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="34"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35"/>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="36"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="20"/>
       <c r="S42" s="3"/>
     </row>
     <row r="43" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C43" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="46" t="s">
+      <c r="D43" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
       <c r="J43" s="4"/>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
@@ -3458,97 +3974,97 @@
       <c r="J47" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K47" s="52" t="s">
+      <c r="K47" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="L47" s="53"/>
-      <c r="M47" s="53"/>
-      <c r="N47" s="53"/>
-      <c r="O47" s="53"/>
-      <c r="P47" s="53"/>
-      <c r="Q47" s="53"/>
-      <c r="R47" s="53"/>
-      <c r="S47" s="54"/>
+      <c r="L47" s="64"/>
+      <c r="M47" s="64"/>
+      <c r="N47" s="64"/>
+      <c r="O47" s="64"/>
+      <c r="P47" s="64"/>
+      <c r="Q47" s="64"/>
+      <c r="R47" s="64"/>
+      <c r="S47" s="65"/>
     </row>
     <row r="48" spans="3:19" x14ac:dyDescent="0.25">
       <c r="J48" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K48" s="55" t="s">
+      <c r="K48" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="L48" s="55"/>
-      <c r="M48" s="55"/>
-      <c r="N48" s="55"/>
-      <c r="O48" s="55"/>
-      <c r="P48" s="55"/>
-      <c r="Q48" s="55"/>
-      <c r="R48" s="55"/>
-      <c r="S48" s="16"/>
+      <c r="L48" s="66"/>
+      <c r="M48" s="66"/>
+      <c r="N48" s="66"/>
+      <c r="O48" s="66"/>
+      <c r="P48" s="66"/>
+      <c r="Q48" s="66"/>
+      <c r="R48" s="66"/>
+      <c r="S48" s="12"/>
     </row>
     <row r="49" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="J49" s="26" t="s">
+      <c r="J49" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="K49" s="17"/>
-      <c r="L49" s="18"/>
-      <c r="M49" s="18"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="19"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="45"/>
+      <c r="M49" s="45"/>
+      <c r="N49" s="45"/>
+      <c r="O49" s="45"/>
+      <c r="P49" s="45"/>
+      <c r="Q49" s="45"/>
+      <c r="R49" s="45"/>
+      <c r="S49" s="46"/>
     </row>
     <row r="50" spans="3:19" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C50" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D50" s="44" t="s">
+      <c r="D50" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="E50" s="44"/>
-      <c r="F50" s="45"/>
-      <c r="J50" s="27"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="21"/>
-      <c r="M50" s="21"/>
-      <c r="N50" s="21"/>
-      <c r="O50" s="21"/>
-      <c r="P50" s="21"/>
-      <c r="Q50" s="21"/>
-      <c r="R50" s="21"/>
-      <c r="S50" s="22"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="58"/>
+      <c r="J50" s="54"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="48"/>
+      <c r="M50" s="48"/>
+      <c r="N50" s="48"/>
+      <c r="O50" s="48"/>
+      <c r="P50" s="48"/>
+      <c r="Q50" s="48"/>
+      <c r="R50" s="48"/>
+      <c r="S50" s="49"/>
     </row>
     <row r="51" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C51" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="39" t="s">
+      <c r="D51" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E51" s="39"/>
-      <c r="F51" s="40"/>
-      <c r="J51" s="28"/>
-      <c r="K51" s="23"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="24"/>
-      <c r="O51" s="24"/>
-      <c r="P51" s="24"/>
-      <c r="Q51" s="24"/>
-      <c r="R51" s="24"/>
-      <c r="S51" s="25"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="24"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="51"/>
+      <c r="M51" s="51"/>
+      <c r="N51" s="51"/>
+      <c r="O51" s="51"/>
+      <c r="P51" s="51"/>
+      <c r="Q51" s="51"/>
+      <c r="R51" s="51"/>
+      <c r="S51" s="52"/>
     </row>
     <row r="52" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C52" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="37" t="s">
+      <c r="D52" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="37"/>
-      <c r="F52" s="38"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="22"/>
       <c r="J52" s="1"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
@@ -3564,25 +4080,25 @@
       <c r="C53" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="47" t="s">
+      <c r="D53" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
       <c r="J53" s="1"/>
-      <c r="K53" s="29"/>
-      <c r="L53" s="30"/>
-      <c r="M53" s="30"/>
-      <c r="N53" s="30"/>
-      <c r="O53" s="30"/>
-      <c r="P53" s="30"/>
-      <c r="Q53" s="30"/>
-      <c r="R53" s="31"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="14"/>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="15"/>
       <c r="S53" s="3"/>
     </row>
     <row r="54" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="J54" s="1"/>
-      <c r="K54" s="32"/>
+      <c r="K54" s="16"/>
       <c r="L54" s="2" t="s">
         <v>27</v>
       </c>
@@ -3591,57 +4107,57 @@
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
-      <c r="R54" s="33"/>
+      <c r="R54" s="17"/>
       <c r="S54" s="3"/>
     </row>
     <row r="55" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="J55" s="1"/>
-      <c r="K55" s="32"/>
+      <c r="K55" s="16"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
-      <c r="R55" s="33"/>
+      <c r="R55" s="17"/>
       <c r="S55" s="3"/>
     </row>
     <row r="56" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="J56" s="1"/>
-      <c r="K56" s="32"/>
-      <c r="L56" s="41" t="s">
+      <c r="K56" s="16"/>
+      <c r="L56" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="M56" s="42"/>
+      <c r="M56" s="26"/>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
-      <c r="Q56" s="49" t="s">
+      <c r="Q56" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="R56" s="33"/>
+      <c r="R56" s="17"/>
       <c r="S56" s="3"/>
     </row>
     <row r="57" spans="3:19" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="58"/>
-      <c r="D57" s="59"/>
-      <c r="E57" s="59"/>
-      <c r="F57" s="59"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="68"/>
+      <c r="F57" s="68"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="34"/>
-      <c r="L57" s="35"/>
-      <c r="M57" s="35"/>
-      <c r="N57" s="35"/>
-      <c r="O57" s="35"/>
-      <c r="P57" s="35"/>
-      <c r="Q57" s="35"/>
-      <c r="R57" s="36"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="19"/>
+      <c r="M57" s="19"/>
+      <c r="N57" s="19"/>
+      <c r="O57" s="19"/>
+      <c r="P57" s="19"/>
+      <c r="Q57" s="19"/>
+      <c r="R57" s="20"/>
       <c r="S57" s="3"/>
     </row>
     <row r="58" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="58"/>
-      <c r="D58" s="60"/>
-      <c r="E58" s="60"/>
-      <c r="F58" s="60"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
       <c r="J58" s="1"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
@@ -3654,13 +4170,13 @@
       <c r="S58" s="3"/>
     </row>
     <row r="59" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="58"/>
-      <c r="D59" s="61"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="61"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
       <c r="J59" s="1"/>
       <c r="K59" s="2"/>
-      <c r="M59" s="42"/>
+      <c r="M59" s="26"/>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
@@ -3669,18 +4185,18 @@
       <c r="S59" s="3"/>
     </row>
     <row r="60" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="58"/>
-      <c r="D60" s="62"/>
-      <c r="E60" s="63"/>
-      <c r="F60" s="63"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
       <c r="J60" s="1"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
-      <c r="N60" s="50" t="s">
+      <c r="N60" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="O60" s="50"/>
+      <c r="O60" s="61"/>
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
@@ -3700,19 +4216,19 @@
     </row>
     <row r="62" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="J62" s="1"/>
-      <c r="K62" s="29"/>
-      <c r="L62" s="30"/>
-      <c r="M62" s="30"/>
-      <c r="N62" s="30"/>
-      <c r="O62" s="30"/>
-      <c r="P62" s="30"/>
-      <c r="Q62" s="30"/>
-      <c r="R62" s="31"/>
+      <c r="K62" s="13"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="14"/>
+      <c r="N62" s="14"/>
+      <c r="O62" s="14"/>
+      <c r="P62" s="14"/>
+      <c r="Q62" s="14"/>
+      <c r="R62" s="15"/>
       <c r="S62" s="3"/>
     </row>
     <row r="63" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="J63" s="1"/>
-      <c r="K63" s="32"/>
+      <c r="K63" s="16"/>
       <c r="L63" s="2" t="s">
         <v>31</v>
       </c>
@@ -3721,12 +4237,12 @@
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
-      <c r="R63" s="33"/>
+      <c r="R63" s="17"/>
       <c r="S63" s="3"/>
     </row>
     <row r="64" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="J64" s="1"/>
-      <c r="K64" s="32"/>
+      <c r="K64" s="16"/>
       <c r="L64" s="2" t="s">
         <v>49</v>
       </c>
@@ -3737,89 +4253,89 @@
         <v>48</v>
       </c>
       <c r="Q64" s="2"/>
-      <c r="R64" s="33"/>
+      <c r="R64" s="17"/>
       <c r="S64" s="3"/>
     </row>
     <row r="65" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="J65" s="1"/>
-      <c r="K65" s="32"/>
-      <c r="M65" s="42"/>
+      <c r="K65" s="16"/>
+      <c r="M65" s="26"/>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
-      <c r="R65" s="33"/>
+      <c r="R65" s="17"/>
       <c r="S65" s="3"/>
     </row>
     <row r="66" spans="3:19" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C66" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D66" s="44" t="s">
+      <c r="D66" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="E66" s="44"/>
-      <c r="F66" s="45"/>
+      <c r="E66" s="57"/>
+      <c r="F66" s="58"/>
       <c r="J66" s="1"/>
-      <c r="K66" s="32"/>
+      <c r="K66" s="16"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="P66" s="2"/>
-      <c r="Q66" s="41" t="s">
+      <c r="Q66" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="R66" s="33"/>
+      <c r="R66" s="17"/>
       <c r="S66" s="3"/>
     </row>
     <row r="67" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C67" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="39" t="s">
+      <c r="D67" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E67" s="39"/>
-      <c r="F67" s="40"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="24"/>
       <c r="J67" s="1"/>
-      <c r="K67" s="32"/>
+      <c r="K67" s="16"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
-      <c r="R67" s="33"/>
+      <c r="R67" s="17"/>
       <c r="S67" s="3"/>
     </row>
     <row r="68" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C68" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="37" t="s">
+      <c r="D68" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E68" s="37"/>
-      <c r="F68" s="38"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="22"/>
       <c r="J68" s="1"/>
-      <c r="K68" s="34"/>
-      <c r="L68" s="35"/>
-      <c r="M68" s="35"/>
-      <c r="N68" s="35"/>
-      <c r="O68" s="35"/>
-      <c r="P68" s="35"/>
-      <c r="Q68" s="35"/>
-      <c r="R68" s="36"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="19"/>
+      <c r="M68" s="19"/>
+      <c r="N68" s="19"/>
+      <c r="O68" s="19"/>
+      <c r="P68" s="19"/>
+      <c r="Q68" s="19"/>
+      <c r="R68" s="20"/>
       <c r="S68" s="3"/>
     </row>
     <row r="69" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C69" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D69" s="46" t="s">
+      <c r="D69" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
       <c r="J69" s="1"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
@@ -3838,11 +4354,11 @@
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
-      <c r="P70" s="51" t="s">
+      <c r="P70" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="Q70" s="51"/>
-      <c r="R70" s="51"/>
+      <c r="Q70" s="56"/>
+      <c r="R70" s="56"/>
       <c r="S70" s="3"/>
     </row>
     <row r="71" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3864,105 +4380,105 @@
       <c r="J75" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K75" s="52" t="s">
+      <c r="K75" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="L75" s="53"/>
-      <c r="M75" s="53"/>
-      <c r="N75" s="53"/>
-      <c r="O75" s="53"/>
-      <c r="P75" s="53"/>
-      <c r="Q75" s="53"/>
-      <c r="R75" s="53"/>
-      <c r="S75" s="54"/>
+      <c r="L75" s="64"/>
+      <c r="M75" s="64"/>
+      <c r="N75" s="64"/>
+      <c r="O75" s="64"/>
+      <c r="P75" s="64"/>
+      <c r="Q75" s="64"/>
+      <c r="R75" s="64"/>
+      <c r="S75" s="65"/>
     </row>
     <row r="76" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="J76" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K76" s="55" t="s">
+      <c r="K76" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="L76" s="55"/>
-      <c r="M76" s="55"/>
-      <c r="N76" s="55"/>
-      <c r="O76" s="55"/>
-      <c r="P76" s="55"/>
-      <c r="Q76" s="55"/>
-      <c r="R76" s="55"/>
-      <c r="S76" s="56"/>
+      <c r="L76" s="66"/>
+      <c r="M76" s="66"/>
+      <c r="N76" s="66"/>
+      <c r="O76" s="66"/>
+      <c r="P76" s="66"/>
+      <c r="Q76" s="66"/>
+      <c r="R76" s="66"/>
+      <c r="S76" s="67"/>
     </row>
     <row r="77" spans="3:19" ht="15.75" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C77" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D77" s="44" t="s">
+      <c r="D77" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="E77" s="44"/>
-      <c r="F77" s="45"/>
-      <c r="J77" s="26" t="s">
+      <c r="E77" s="57"/>
+      <c r="F77" s="58"/>
+      <c r="J77" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="K77" s="17"/>
-      <c r="L77" s="18"/>
-      <c r="M77" s="18"/>
-      <c r="N77" s="18"/>
-      <c r="O77" s="18"/>
-      <c r="P77" s="18"/>
-      <c r="Q77" s="18"/>
-      <c r="R77" s="18"/>
-      <c r="S77" s="19"/>
+      <c r="K77" s="44"/>
+      <c r="L77" s="45"/>
+      <c r="M77" s="45"/>
+      <c r="N77" s="45"/>
+      <c r="O77" s="45"/>
+      <c r="P77" s="45"/>
+      <c r="Q77" s="45"/>
+      <c r="R77" s="45"/>
+      <c r="S77" s="46"/>
     </row>
     <row r="78" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C78" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D78" s="39" t="s">
+      <c r="D78" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E78" s="39"/>
-      <c r="F78" s="40"/>
-      <c r="J78" s="27"/>
-      <c r="K78" s="20"/>
-      <c r="L78" s="21"/>
-      <c r="M78" s="21"/>
-      <c r="N78" s="21"/>
-      <c r="O78" s="21"/>
-      <c r="P78" s="21"/>
-      <c r="Q78" s="21"/>
-      <c r="R78" s="21"/>
-      <c r="S78" s="22"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="24"/>
+      <c r="J78" s="54"/>
+      <c r="K78" s="47"/>
+      <c r="L78" s="48"/>
+      <c r="M78" s="48"/>
+      <c r="N78" s="48"/>
+      <c r="O78" s="48"/>
+      <c r="P78" s="48"/>
+      <c r="Q78" s="48"/>
+      <c r="R78" s="48"/>
+      <c r="S78" s="49"/>
     </row>
     <row r="79" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C79" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D79" s="37" t="s">
+      <c r="D79" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E79" s="37"/>
-      <c r="F79" s="38"/>
-      <c r="J79" s="28"/>
-      <c r="K79" s="23"/>
-      <c r="L79" s="24"/>
-      <c r="M79" s="24"/>
-      <c r="N79" s="24"/>
-      <c r="O79" s="24"/>
-      <c r="P79" s="24"/>
-      <c r="Q79" s="24"/>
-      <c r="R79" s="24"/>
-      <c r="S79" s="25"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="22"/>
+      <c r="J79" s="55"/>
+      <c r="K79" s="50"/>
+      <c r="L79" s="51"/>
+      <c r="M79" s="51"/>
+      <c r="N79" s="51"/>
+      <c r="O79" s="51"/>
+      <c r="P79" s="51"/>
+      <c r="Q79" s="51"/>
+      <c r="R79" s="51"/>
+      <c r="S79" s="52"/>
     </row>
     <row r="80" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C80" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D80" s="46" t="s">
+      <c r="D80" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
       <c r="J80" s="1"/>
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
@@ -3976,23 +4492,23 @@
     </row>
     <row r="81" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="J81" s="1"/>
-      <c r="K81" s="29"/>
-      <c r="L81" s="30"/>
-      <c r="M81" s="30"/>
-      <c r="N81" s="30"/>
-      <c r="O81" s="30"/>
-      <c r="P81" s="30"/>
-      <c r="Q81" s="30"/>
-      <c r="R81" s="31"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="14"/>
+      <c r="N81" s="14"/>
+      <c r="O81" s="14"/>
+      <c r="P81" s="14"/>
+      <c r="Q81" s="14"/>
+      <c r="R81" s="15"/>
       <c r="S81" s="3"/>
     </row>
     <row r="82" spans="3:19" ht="15.75" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C82" s="58"/>
-      <c r="D82" s="67"/>
-      <c r="E82" s="67"/>
-      <c r="F82" s="67"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="40"/>
+      <c r="E82" s="40"/>
+      <c r="F82" s="40"/>
       <c r="J82" s="1"/>
-      <c r="K82" s="32"/>
+      <c r="K82" s="16"/>
       <c r="L82" s="2" t="s">
         <v>49</v>
       </c>
@@ -4003,56 +4519,56 @@
         <v>48</v>
       </c>
       <c r="Q82" s="2"/>
-      <c r="R82" s="33"/>
+      <c r="R82" s="17"/>
       <c r="S82" s="3"/>
     </row>
     <row r="83" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C83" s="58"/>
-      <c r="D83" s="60"/>
-      <c r="E83" s="60"/>
-      <c r="F83" s="60"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="34"/>
+      <c r="F83" s="34"/>
       <c r="J83" s="1"/>
-      <c r="K83" s="32"/>
+      <c r="K83" s="16"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
       <c r="P83" s="2"/>
       <c r="Q83" s="2"/>
-      <c r="R83" s="33"/>
+      <c r="R83" s="17"/>
       <c r="S83" s="3"/>
     </row>
     <row r="84" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C84" s="58"/>
-      <c r="D84" s="61"/>
-      <c r="E84" s="61"/>
-      <c r="F84" s="61"/>
+      <c r="C84" s="33"/>
+      <c r="D84" s="35"/>
+      <c r="E84" s="35"/>
+      <c r="F84" s="35"/>
       <c r="J84" s="1"/>
-      <c r="K84" s="32"/>
-      <c r="M84" s="42"/>
-      <c r="O84" s="41" t="s">
+      <c r="K84" s="16"/>
+      <c r="M84" s="26"/>
+      <c r="O84" s="25" t="s">
         <v>34</v>
       </c>
       <c r="P84" s="2"/>
-      <c r="Q84" s="41" t="s">
+      <c r="Q84" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="R84" s="33"/>
+      <c r="R84" s="17"/>
       <c r="S84" s="3"/>
     </row>
     <row r="85" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C85" s="58"/>
-      <c r="D85" s="62"/>
-      <c r="E85" s="63"/>
-      <c r="F85" s="63"/>
+      <c r="C85" s="33"/>
+      <c r="D85" s="36"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="37"/>
       <c r="J85" s="1"/>
-      <c r="K85" s="34"/>
-      <c r="L85" s="35"/>
-      <c r="M85" s="35"/>
-      <c r="N85" s="35"/>
-      <c r="O85" s="35"/>
-      <c r="P85" s="35"/>
-      <c r="Q85" s="35"/>
-      <c r="R85" s="36"/>
+      <c r="K85" s="18"/>
+      <c r="L85" s="19"/>
+      <c r="M85" s="19"/>
+      <c r="N85" s="19"/>
+      <c r="O85" s="19"/>
+      <c r="P85" s="19"/>
+      <c r="Q85" s="19"/>
+      <c r="R85" s="20"/>
       <c r="S85" s="3"/>
     </row>
     <row r="86" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4069,19 +4585,19 @@
     </row>
     <row r="87" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="J87" s="1"/>
-      <c r="K87" s="29"/>
-      <c r="L87" s="30"/>
-      <c r="M87" s="30"/>
-      <c r="N87" s="30"/>
-      <c r="O87" s="30"/>
-      <c r="P87" s="30"/>
-      <c r="Q87" s="30"/>
-      <c r="R87" s="31"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="14"/>
+      <c r="M87" s="14"/>
+      <c r="N87" s="14"/>
+      <c r="O87" s="14"/>
+      <c r="P87" s="14"/>
+      <c r="Q87" s="14"/>
+      <c r="R87" s="15"/>
       <c r="S87" s="3"/>
     </row>
     <row r="88" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="J88" s="1"/>
-      <c r="K88" s="32"/>
+      <c r="K88" s="16"/>
       <c r="L88" t="s">
         <v>40</v>
       </c>
@@ -4090,256 +4606,256 @@
       <c r="O88" s="2"/>
       <c r="P88" s="2"/>
       <c r="Q88" s="2"/>
-      <c r="R88" s="33"/>
+      <c r="R88" s="17"/>
       <c r="S88" s="3"/>
     </row>
     <row r="89" spans="3:19" ht="15.75" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C89" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D89" s="44" t="s">
+      <c r="D89" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="E89" s="44"/>
-      <c r="F89" s="45"/>
+      <c r="E89" s="57"/>
+      <c r="F89" s="58"/>
       <c r="J89" s="1"/>
-      <c r="K89" s="32"/>
+      <c r="K89" s="16"/>
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
       <c r="P89" s="2"/>
       <c r="Q89" s="2"/>
-      <c r="R89" s="33"/>
+      <c r="R89" s="17"/>
       <c r="S89" s="3"/>
     </row>
     <row r="90" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C90" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D90" s="39" t="s">
+      <c r="D90" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E90" s="39"/>
-      <c r="F90" s="40"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="24"/>
       <c r="J90" s="1"/>
-      <c r="K90" s="32"/>
-      <c r="M90" s="42"/>
+      <c r="K90" s="16"/>
+      <c r="M90" s="26"/>
       <c r="N90" s="2"/>
       <c r="O90" s="2"/>
       <c r="P90" s="2"/>
       <c r="Q90" s="2"/>
-      <c r="R90" s="33"/>
+      <c r="R90" s="17"/>
       <c r="S90" s="3"/>
     </row>
     <row r="91" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C91" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D91" s="37" t="s">
+      <c r="D91" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E91" s="37"/>
-      <c r="F91" s="38"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="22"/>
       <c r="G91" s="2"/>
       <c r="J91" s="1"/>
-      <c r="K91" s="32"/>
+      <c r="K91" s="16"/>
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
-      <c r="R91" s="33"/>
+      <c r="R91" s="17"/>
       <c r="S91" s="3"/>
     </row>
     <row r="92" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C92" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D92" s="47" t="s">
+      <c r="D92" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
       <c r="J92" s="1"/>
-      <c r="K92" s="32"/>
+      <c r="K92" s="16"/>
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
-      <c r="O92" s="41" t="s">
+      <c r="O92" s="25" t="s">
         <v>37</v>
       </c>
       <c r="P92" s="2"/>
-      <c r="Q92" s="49" t="s">
+      <c r="Q92" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="R92" s="33"/>
+      <c r="R92" s="17"/>
       <c r="S92" s="3"/>
     </row>
     <row r="93" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="J93" s="1"/>
-      <c r="K93" s="32"/>
-      <c r="L93" s="51" t="s">
+      <c r="K93" s="16"/>
+      <c r="L93" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="M93" s="51"/>
+      <c r="M93" s="56"/>
       <c r="N93" s="2"/>
       <c r="P93" s="2"/>
-      <c r="Q93" s="57"/>
-      <c r="R93" s="33"/>
+      <c r="Q93" s="32"/>
+      <c r="R93" s="17"/>
       <c r="S93" s="3"/>
     </row>
     <row r="94" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="J94" s="1"/>
-      <c r="K94" s="34"/>
-      <c r="L94" s="35"/>
-      <c r="M94" s="35"/>
-      <c r="N94" s="35"/>
-      <c r="O94" s="35"/>
-      <c r="P94" s="35"/>
-      <c r="Q94" s="35"/>
-      <c r="R94" s="36"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="19"/>
+      <c r="M94" s="19"/>
+      <c r="N94" s="19"/>
+      <c r="O94" s="19"/>
+      <c r="P94" s="19"/>
+      <c r="Q94" s="19"/>
+      <c r="R94" s="20"/>
       <c r="S94" s="3"/>
     </row>
     <row r="95" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="J95" s="1"/>
-      <c r="K95" s="32"/>
+      <c r="K95" s="16"/>
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
       <c r="P95" s="2"/>
-      <c r="Q95" s="57"/>
-      <c r="R95" s="33"/>
+      <c r="Q95" s="32"/>
+      <c r="R95" s="17"/>
       <c r="S95" s="3"/>
     </row>
     <row r="96" spans="3:19" ht="15.75" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C96" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D96" s="44" t="s">
+      <c r="D96" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="E96" s="44"/>
-      <c r="F96" s="45"/>
+      <c r="E96" s="57"/>
+      <c r="F96" s="58"/>
       <c r="J96" s="1"/>
-      <c r="K96" s="32"/>
+      <c r="K96" s="16"/>
       <c r="L96" s="2" t="s">
         <v>41</v>
       </c>
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
       <c r="P96" s="2"/>
-      <c r="Q96" s="57"/>
-      <c r="R96" s="33"/>
+      <c r="Q96" s="32"/>
+      <c r="R96" s="17"/>
       <c r="S96" s="3"/>
     </row>
     <row r="97" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C97" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D97" s="39" t="s">
+      <c r="D97" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E97" s="39"/>
-      <c r="F97" s="40"/>
-      <c r="G97" s="64"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="38"/>
       <c r="J97" s="1"/>
-      <c r="K97" s="32"/>
+      <c r="K97" s="16"/>
       <c r="L97" s="2"/>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
       <c r="P97" s="2"/>
-      <c r="Q97" s="57"/>
-      <c r="R97" s="33"/>
+      <c r="Q97" s="32"/>
+      <c r="R97" s="17"/>
       <c r="S97" s="3"/>
     </row>
     <row r="98" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C98" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D98" s="37" t="s">
+      <c r="D98" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E98" s="37"/>
-      <c r="F98" s="38"/>
-      <c r="G98" s="65"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="22"/>
+      <c r="G98" s="39"/>
       <c r="J98" s="1"/>
-      <c r="K98" s="32"/>
+      <c r="K98" s="16"/>
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
       <c r="P98" s="2"/>
-      <c r="Q98" s="57"/>
-      <c r="R98" s="33"/>
+      <c r="Q98" s="32"/>
+      <c r="R98" s="17"/>
       <c r="S98" s="3"/>
     </row>
     <row r="99" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="C99" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D99" s="47" t="s">
+      <c r="D99" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E99" s="11"/>
-      <c r="F99" s="11"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
       <c r="J99" s="1"/>
-      <c r="K99" s="32"/>
-      <c r="L99" s="51" t="s">
+      <c r="K99" s="16"/>
+      <c r="L99" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="M99" s="51"/>
+      <c r="M99" s="56"/>
       <c r="N99" s="2"/>
       <c r="P99" s="2"/>
-      <c r="Q99" s="41" t="s">
+      <c r="Q99" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="R99" s="33"/>
+      <c r="R99" s="17"/>
       <c r="S99" s="3"/>
     </row>
     <row r="100" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="J100" s="1"/>
-      <c r="K100" s="32"/>
+      <c r="K100" s="16"/>
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
       <c r="P100" s="2"/>
-      <c r="Q100" s="57"/>
-      <c r="R100" s="33"/>
+      <c r="Q100" s="32"/>
+      <c r="R100" s="17"/>
       <c r="S100" s="3"/>
     </row>
     <row r="101" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="J101" s="1"/>
-      <c r="K101" s="32"/>
+      <c r="K101" s="16"/>
       <c r="L101" s="2"/>
       <c r="M101" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N101" s="2"/>
       <c r="P101" s="2"/>
-      <c r="Q101" s="57"/>
-      <c r="R101" s="33"/>
+      <c r="Q101" s="32"/>
+      <c r="R101" s="17"/>
       <c r="S101" s="3"/>
     </row>
     <row r="102" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="J102" s="1"/>
-      <c r="K102" s="32"/>
+      <c r="K102" s="16"/>
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
-      <c r="R102" s="33"/>
+      <c r="R102" s="17"/>
       <c r="S102" s="3"/>
     </row>
     <row r="103" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="J103" s="1"/>
-      <c r="K103" s="34"/>
-      <c r="L103" s="35"/>
-      <c r="M103" s="35"/>
-      <c r="N103" s="35"/>
-      <c r="O103" s="35"/>
-      <c r="P103" s="35"/>
-      <c r="Q103" s="35"/>
-      <c r="R103" s="36"/>
+      <c r="K103" s="18"/>
+      <c r="L103" s="19"/>
+      <c r="M103" s="19"/>
+      <c r="N103" s="19"/>
+      <c r="O103" s="19"/>
+      <c r="P103" s="19"/>
+      <c r="Q103" s="19"/>
+      <c r="R103" s="20"/>
       <c r="S103" s="3"/>
     </row>
     <row r="104" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4353,10 +4869,10 @@
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
-      <c r="Q105" s="51" t="s">
+      <c r="Q105" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="R105" s="51"/>
+      <c r="R105" s="56"/>
       <c r="S105" s="3"/>
     </row>
     <row r="106" spans="3:19" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4372,12 +4888,160 @@
       <c r="S106" s="6"/>
     </row>
     <row r="107" spans="3:19" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="E108" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="E109" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q109" s="43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="112" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="L112" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="113" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N113" s="42"/>
+    </row>
+    <row r="114" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="K114" s="13"/>
+      <c r="L114" s="14"/>
+      <c r="M114" s="14"/>
+      <c r="N114" s="14"/>
+      <c r="O114" s="14"/>
+      <c r="P114" s="14"/>
+      <c r="Q114" s="41"/>
+      <c r="R114" s="15"/>
+    </row>
+    <row r="115" spans="3:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C115" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E115" s="57"/>
+      <c r="F115" s="58"/>
+      <c r="K115" s="16"/>
+      <c r="L115" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M115" s="2"/>
+      <c r="N115" s="2"/>
+      <c r="O115" s="2"/>
+      <c r="P115" s="2"/>
+      <c r="Q115" s="32"/>
+      <c r="R115" s="17"/>
+    </row>
+    <row r="116" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C116" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D116" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E116" s="23"/>
+      <c r="F116" s="24"/>
+      <c r="K116" s="16"/>
+      <c r="L116" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M116" s="2"/>
+      <c r="N116" s="2"/>
+      <c r="O116" s="2"/>
+      <c r="P116" s="2"/>
+      <c r="Q116" s="32"/>
+      <c r="R116" s="17"/>
+    </row>
+    <row r="117" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C117" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D117" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E117" s="21"/>
+      <c r="F117" s="22"/>
+      <c r="K117" s="16"/>
+      <c r="L117" s="2"/>
+      <c r="M117" s="2"/>
+      <c r="N117" s="2"/>
+      <c r="O117" s="2"/>
+      <c r="P117" s="2"/>
+      <c r="Q117" s="32"/>
+      <c r="R117" s="17"/>
+    </row>
+    <row r="118" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C118" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D118" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9"/>
+      <c r="K118" s="16"/>
+      <c r="M118" s="2"/>
+      <c r="N118" s="2"/>
+      <c r="O118" s="2"/>
+      <c r="P118" s="2"/>
+      <c r="R118" s="17"/>
+    </row>
+    <row r="119" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="K119" s="16"/>
+      <c r="L119" s="2"/>
+      <c r="M119" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="N119" s="56"/>
+      <c r="O119" s="56"/>
+      <c r="P119" s="2"/>
+      <c r="Q119" s="32"/>
+      <c r="R119" s="17"/>
+    </row>
+    <row r="120" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="K120" s="16"/>
+      <c r="L120" t="s">
+        <v>58</v>
+      </c>
+      <c r="N120" s="2"/>
+      <c r="O120" s="2"/>
+      <c r="P120" s="2"/>
+      <c r="Q120" s="32"/>
+      <c r="R120" s="17"/>
+    </row>
+    <row r="121" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="K121" s="16"/>
+      <c r="L121" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M121" s="2"/>
+      <c r="N121" s="2"/>
+      <c r="O121" s="2"/>
+      <c r="P121" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q121" s="56"/>
+      <c r="R121" s="17"/>
+    </row>
+    <row r="122" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="K122" s="18"/>
+      <c r="L122" s="19"/>
+      <c r="M122" s="19"/>
+      <c r="N122" s="19"/>
+      <c r="O122" s="19"/>
+      <c r="P122" s="19"/>
+      <c r="Q122" s="19"/>
+      <c r="R122" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="L99:M99"/>
-    <mergeCell ref="D77:F77"/>
-    <mergeCell ref="D89:F89"/>
-    <mergeCell ref="D96:F96"/>
+  <mergeCells count="33">
     <mergeCell ref="B3:D5"/>
     <mergeCell ref="J77:J79"/>
     <mergeCell ref="K77:S79"/>
@@ -4385,28 +5049,35 @@
     <mergeCell ref="K48:R48"/>
     <mergeCell ref="K75:S75"/>
     <mergeCell ref="K76:S76"/>
-    <mergeCell ref="L93:M93"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D17:F17"/>
     <mergeCell ref="Q105:R105"/>
     <mergeCell ref="J49:J51"/>
     <mergeCell ref="K49:S51"/>
     <mergeCell ref="N60:O60"/>
     <mergeCell ref="P70:R70"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D66:F66"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="D77:F77"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="L93:M93"/>
+    <mergeCell ref="K17:S19"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="P121:Q121"/>
+    <mergeCell ref="M119:O119"/>
+    <mergeCell ref="D115:F115"/>
     <mergeCell ref="D40:F40"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="K17:S19"/>
-    <mergeCell ref="J17:J19"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12 D99 D92 D85 D80 D69 D60 D53 D43 D34 D27 D20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12 D99 D92 D85 D80 D69 D60 D53 D43 D34 D27 D20 D118">
       <formula1>$AA$13:$AA$14</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>